<commit_message>
Test no volume ksvmeans
</commit_message>
<xml_diff>
--- a/Document/TestResult.xlsx
+++ b/Document/TestResult.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="7740"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="7740" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ANN" sheetId="1" r:id="rId1"/>
@@ -427,7 +427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -596,7 +596,7 @@
   <dimension ref="A2:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -773,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -818,6 +818,9 @@
       <c r="E4">
         <v>66.430000000000007</v>
       </c>
+      <c r="F4">
+        <v>59.42</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
@@ -832,6 +835,9 @@
       <c r="E5">
         <v>56.98</v>
       </c>
+      <c r="F5">
+        <v>55.67</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
@@ -846,6 +852,9 @@
       <c r="E6">
         <v>69.14</v>
       </c>
+      <c r="F6" s="4">
+        <v>51.87</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
@@ -860,6 +869,9 @@
       <c r="E7">
         <v>62.16</v>
       </c>
+      <c r="F7">
+        <v>57.61</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
@@ -873,6 +885,9 @@
       </c>
       <c r="E8" s="4">
         <v>58.19</v>
+      </c>
+      <c r="F8">
+        <v>55.84</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -891,6 +906,10 @@
       <c r="E9" s="2">
         <f>AVERAGE(E4:E8)</f>
         <v>62.58</v>
+      </c>
+      <c r="F9" s="2">
+        <f>AVERAGE(F4:F8)</f>
+        <v>56.081999999999994</v>
       </c>
     </row>
   </sheetData>
@@ -899,5 +918,6 @@
     <mergeCell ref="E2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Kết quả test Với đầu vào có và ko có Volumes
</commit_message>
<xml_diff>
--- a/Document/TestResult.xlsx
+++ b/Document/TestResult.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="7740" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="ANN" sheetId="1" r:id="rId1"/>
     <sheet name="SVM" sheetId="2" r:id="rId2"/>
     <sheet name="K-SVMeans" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="17">
   <si>
     <t>period = 1</t>
   </si>
@@ -61,13 +61,19 @@
   </si>
   <si>
     <t>Aroon = 10</t>
+  </si>
+  <si>
+    <t>ANN.NET Volume</t>
+  </si>
+  <si>
+    <t>ANN.NET NoVolume</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,6 +221,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -249,6 +256,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -424,14 +432,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -439,24 +447,31 @@
     <col min="8" max="8" width="12.28515625" customWidth="1"/>
     <col min="9" max="9" width="14.85546875" customWidth="1"/>
     <col min="10" max="10" width="10.5703125" customWidth="1"/>
-    <col min="11" max="11" width="6.85546875" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" customWidth="1"/>
     <col min="12" max="12" width="13.7109375" customWidth="1"/>
     <col min="13" max="13" width="14.85546875" customWidth="1"/>
     <col min="14" max="14" width="10.42578125" customWidth="1"/>
     <col min="15" max="15" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
+      <c r="G1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -469,8 +484,20 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -486,8 +513,23 @@
       <c r="E3">
         <v>58.45</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="I3">
+        <v>67.78</v>
+      </c>
+      <c r="J3">
+        <v>59.33</v>
+      </c>
+      <c r="K3">
+        <v>41.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -500,8 +542,23 @@
       <c r="E4">
         <v>55.55</v>
       </c>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>56.98</v>
+      </c>
+      <c r="I4">
+        <v>56.75</v>
+      </c>
+      <c r="J4">
+        <v>56.52</v>
+      </c>
+      <c r="K4">
+        <v>47.22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -517,8 +574,23 @@
       <c r="E5">
         <v>20.32</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="G5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <v>67.02</v>
+      </c>
+      <c r="I5">
+        <v>32.619999999999997</v>
+      </c>
+      <c r="J5">
+        <v>43.01</v>
+      </c>
+      <c r="K5">
+        <v>47.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -534,8 +606,23 @@
       <c r="E6">
         <v>30.72</v>
       </c>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6">
+        <v>42.16</v>
+      </c>
+      <c r="I6">
+        <v>41.84</v>
+      </c>
+      <c r="J6">
+        <v>51.91</v>
+      </c>
+      <c r="K6">
+        <v>55.86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -548,8 +635,23 @@
       <c r="E7">
         <v>34.950000000000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7">
+        <v>59.05</v>
+      </c>
+      <c r="I7">
+        <v>56.7</v>
+      </c>
+      <c r="J7">
+        <v>54.34</v>
+      </c>
+      <c r="K7">
+        <v>41.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -569,22 +671,165 @@
         <f t="shared" si="0"/>
         <v>39.998000000000005</v>
       </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="2">
+        <f>AVERAGE(H3:H7)</f>
+        <v>58.661999999999992</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" ref="I8:K8" si="1">AVERAGE(I3:I7)</f>
+        <v>51.137999999999998</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>53.022000000000006</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>46.666000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>72.849999999999994</v>
+      </c>
+      <c r="C12">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="D12">
+        <v>44.01</v>
+      </c>
+      <c r="E12">
+        <v>58.45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>56.98</v>
+      </c>
+      <c r="C13">
+        <v>56.75</v>
+      </c>
+      <c r="D13">
+        <v>44.02</v>
+      </c>
+      <c r="E13">
+        <v>31.66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>43.61</v>
+      </c>
+      <c r="C14">
+        <v>60.96</v>
+      </c>
+      <c r="D14">
+        <v>67.2</v>
+      </c>
+      <c r="E14">
+        <v>32.409999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>49.72</v>
+      </c>
+      <c r="C15">
+        <v>38.58</v>
+      </c>
+      <c r="D15">
+        <v>60.65</v>
+      </c>
+      <c r="E15">
+        <v>52.51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>56.46</v>
+      </c>
+      <c r="C16">
+        <v>57.14</v>
+      </c>
+      <c r="D16">
+        <v>50</v>
+      </c>
+      <c r="E16">
+        <v>37.61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2">
+        <f>AVERAGE(B12:B16)</f>
+        <v>55.923999999999999</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" ref="C17:E17" si="2">AVERAGE(C12:C16)</f>
+        <v>55.905999999999992</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>53.176000000000002</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>42.527999999999999</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="A10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -592,20 +837,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="17.140625" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
@@ -617,7 +862,7 @@
       </c>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -634,7 +879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -654,7 +899,7 @@
         <v>60.95</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -674,7 +919,7 @@
         <v>56.98</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -694,7 +939,7 @@
         <v>70.209999999999994</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -714,7 +959,7 @@
         <v>56.21</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -734,7 +979,7 @@
         <v>57.75</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -770,16 +1015,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -791,7 +1036,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -805,7 +1050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -818,11 +1063,8 @@
       <c r="E4">
         <v>66.430000000000007</v>
       </c>
-      <c r="F4">
-        <v>59.42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -835,11 +1077,8 @@
       <c r="E5">
         <v>56.98</v>
       </c>
-      <c r="F5">
-        <v>55.67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -852,11 +1091,8 @@
       <c r="E6">
         <v>69.14</v>
       </c>
-      <c r="F6" s="4">
-        <v>51.87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -869,11 +1105,8 @@
       <c r="E7">
         <v>62.16</v>
       </c>
-      <c r="F7">
-        <v>57.61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -886,11 +1119,8 @@
       <c r="E8" s="4">
         <v>58.19</v>
       </c>
-      <c r="F8">
-        <v>55.84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -906,10 +1136,6 @@
       <c r="E9" s="2">
         <f>AVERAGE(E4:E8)</f>
         <v>62.58</v>
-      </c>
-      <c r="F9" s="2">
-        <f>AVERAGE(F4:F8)</f>
-        <v>56.081999999999994</v>
       </c>
     </row>
   </sheetData>
@@ -918,6 +1144,5 @@
     <mergeCell ref="E2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
test ksvmeans với k = 3
</commit_message>
<xml_diff>
--- a/Document/TestResult.xlsx
+++ b/Document/TestResult.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="7740"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="7740" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ANN" sheetId="1" r:id="rId1"/>
     <sheet name="SVM" sheetId="2" r:id="rId2"/>
     <sheet name="K-SVMeans" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="18">
   <si>
     <t>period = 1</t>
   </si>
@@ -67,13 +67,16 @@
   </si>
   <si>
     <t>ANN.NET NoVolume</t>
+  </si>
+  <si>
+    <t>K= 3, Aroon = 5, No volume</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,7 +224,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -256,7 +258,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -432,14 +433,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -454,7 +455,7 @@
     <col min="15" max="15" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="B1" s="5" t="s">
         <v>11</v>
       </c>
@@ -471,7 +472,7 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -497,7 +498,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -529,7 +530,7 @@
         <v>41.3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -558,7 +559,7 @@
         <v>47.22</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -590,7 +591,7 @@
         <v>47.8</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -622,7 +623,7 @@
         <v>55.86</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -651,7 +652,7 @@
         <v>41.15</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -691,7 +692,7 @@
         <v>46.666000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
@@ -705,7 +706,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="B11" t="s">
         <v>0</v>
       </c>
@@ -719,7 +720,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -736,7 +737,7 @@
         <v>58.45</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -753,7 +754,7 @@
         <v>31.66</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -770,7 +771,7 @@
         <v>32.409999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -787,7 +788,7 @@
         <v>52.51</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -804,7 +805,7 @@
         <v>37.61</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -837,20 +838,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="17.140625" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
@@ -862,7 +863,7 @@
       </c>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -879,7 +880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -899,7 +900,7 @@
         <v>60.95</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -919,7 +920,7 @@
         <v>56.98</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -939,7 +940,7 @@
         <v>70.209999999999994</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -959,7 +960,7 @@
         <v>56.21</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -979,7 +980,7 @@
         <v>57.75</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1015,16 +1016,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -1036,7 +1037,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -1050,7 +1051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1063,8 +1064,11 @@
       <c r="E4">
         <v>66.430000000000007</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>59.42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1077,8 +1081,11 @@
       <c r="E5">
         <v>56.98</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>55.67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1091,8 +1098,11 @@
       <c r="E6">
         <v>69.14</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F6" s="4">
+        <v>51.87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1105,8 +1115,11 @@
       <c r="E7">
         <v>62.16</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>57.61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1119,8 +1132,11 @@
       <c r="E8" s="4">
         <v>58.19</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>55.84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1136,6 +1152,72 @@
       <c r="E9" s="2">
         <f>AVERAGE(E4:E8)</f>
         <v>62.58</v>
+      </c>
+      <c r="F9" s="2">
+        <f>AVERAGE(F4:F8)</f>
+        <v>56.081999999999994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>64.52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="4">
+        <v>59.14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="4">
+        <v>65.95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <v>51.89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>56.89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="2">
+        <f>AVERAGE(B13:B17)</f>
+        <v>59.677999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -1144,5 +1226,6 @@
     <mergeCell ref="E2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bổ sung k = 3
</commit_message>
<xml_diff>
--- a/Document/TestResult.xlsx
+++ b/Document/TestResult.xlsx
@@ -1020,7 +1020,7 @@
   <dimension ref="A2:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1178,6 +1178,9 @@
       <c r="B13">
         <v>64.52</v>
       </c>
+      <c r="C13">
+        <v>58.23</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
@@ -1186,6 +1189,9 @@
       <c r="B14" s="4">
         <v>59.14</v>
       </c>
+      <c r="C14">
+        <v>55.67</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
@@ -1194,6 +1200,9 @@
       <c r="B15" s="4">
         <v>65.95</v>
       </c>
+      <c r="C15">
+        <v>50.26</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
@@ -1202,22 +1211,32 @@
       <c r="B16">
         <v>51.89</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16">
+        <v>54.89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>8</v>
       </c>
       <c r="B17">
         <v>56.89</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17">
+        <v>53.24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="2">
         <f>AVERAGE(B13:B17)</f>
         <v>59.677999999999997</v>
+      </c>
+      <c r="C18" s="2">
+        <f>AVERAGE(C13:C17)</f>
+        <v>54.458000000000006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Up sơ vài kết quả test mới
</commit_message>
<xml_diff>
--- a/Document/TestResult.xlsx
+++ b/Document/TestResult.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="25">
   <si>
     <t>period = 1</t>
   </si>
@@ -70,6 +70,27 @@
   </si>
   <si>
     <t>K= 3, Aroon = 5, No volume</t>
+  </si>
+  <si>
+    <t>Bộ test giới hạn 997 obs từ 4-1-2005 đến 31-12-2008</t>
+  </si>
+  <si>
+    <t>DHA</t>
+  </si>
+  <si>
+    <t>KHA</t>
+  </si>
+  <si>
+    <t>REE</t>
+  </si>
+  <si>
+    <t>SAM</t>
+  </si>
+  <si>
+    <t>SAV</t>
+  </si>
+  <si>
+    <t>Probab, K = 2</t>
   </si>
 </sst>
 </file>
@@ -839,10 +860,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:H9"/>
+  <dimension ref="A2:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A20" sqref="A20:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1005,10 +1026,60 @@
         <v>60.42</v>
       </c>
     </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A18:O18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1017,13 +1088,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:G18"/>
+  <dimension ref="A2:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:7">
       <c r="A2" s="5" t="s">
@@ -1215,7 +1290,7 @@
         <v>54.89</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1226,7 +1301,7 @@
         <v>53.24</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -1239,10 +1314,103 @@
         <v>54.458000000000006</v>
       </c>
     </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="4">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26">
+        <v>82.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="4">
+        <v>75.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="4">
+        <v>60.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29">
+        <f>AVERAGE(B23:B28)</f>
+        <v>69.416666666666671</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="E2:G2"/>
+    <mergeCell ref="A20:O20"/>
+    <mergeCell ref="A21:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Tiếp tục chỉnh sửa paper
</commit_message>
<xml_diff>
--- a/Document/TestResult.xlsx
+++ b/Document/TestResult.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="7740" activeTab="2"/>
@@ -11,7 +11,7 @@
     <sheet name="SVM" sheetId="2" r:id="rId2"/>
     <sheet name="K-SVMeans" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -96,8 +96,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,6 +245,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -279,6 +280,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -454,14 +456,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -476,7 +478,7 @@
     <col min="15" max="15" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
         <v>11</v>
       </c>
@@ -493,7 +495,7 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -519,7 +521,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -551,7 +553,7 @@
         <v>41.3</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -580,7 +582,7 @@
         <v>47.22</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -612,7 +614,7 @@
         <v>47.8</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -644,7 +646,7 @@
         <v>55.86</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -673,7 +675,7 @@
         <v>41.15</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -713,7 +715,7 @@
         <v>46.666000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
@@ -727,7 +729,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>0</v>
       </c>
@@ -741,7 +743,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -758,7 +760,7 @@
         <v>58.45</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -775,7 +777,7 @@
         <v>31.66</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -792,7 +794,7 @@
         <v>32.409999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -809,7 +811,7 @@
         <v>52.51</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -826,7 +828,7 @@
         <v>37.61</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -859,20 +861,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20:A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="17.140625" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
@@ -884,7 +886,7 @@
       </c>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -901,7 +903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -921,7 +923,7 @@
         <v>60.95</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -941,7 +943,7 @@
         <v>56.98</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -961,7 +963,7 @@
         <v>70.209999999999994</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -981,7 +983,7 @@
         <v>56.21</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1001,7 +1003,7 @@
         <v>57.75</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1026,7 +1028,7 @@
         <v>60.42</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1045,32 +1047,32 @@
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1087,20 +1089,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.140625" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -1112,7 +1114,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -1126,7 +1128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1143,7 +1145,7 @@
         <v>59.42</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1160,7 +1162,7 @@
         <v>55.67</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1177,7 +1179,7 @@
         <v>51.87</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1194,7 +1196,7 @@
         <v>57.61</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1211,7 +1213,7 @@
         <v>55.84</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1233,12 +1235,12 @@
         <v>56.081999999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>0</v>
       </c>
@@ -1246,7 +1248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1257,7 +1259,7 @@
         <v>58.23</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1268,7 +1270,7 @@
         <v>55.67</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1279,7 +1281,7 @@
         <v>50.26</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1290,7 +1292,7 @@
         <v>54.89</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1301,7 +1303,7 @@
         <v>53.24</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -1314,7 +1316,7 @@
         <v>54.458000000000006</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>18</v>
       </c>
@@ -1333,14 +1335,14 @@
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>0</v>
       </c>
@@ -1348,7 +1350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1356,7 +1358,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -1364,7 +1366,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -1372,7 +1374,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1380,7 +1382,7 @@
         <v>82.5</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -1388,7 +1390,7 @@
         <v>75.5</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -1396,7 +1398,7 @@
         <v>60.5</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>

</xml_diff>